<commit_message>
Actualización V3 con la explicación del profe
</commit_message>
<xml_diff>
--- a/tablas.xlsx
+++ b/tablas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1655775e314bd799/Maestría IA Aplicada/Semestre 1/Aprendizaje automático III/Talleres/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1D44CD4-F765-41BB-8147-D381176485D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{B1D44CD4-F765-41BB-8147-D381176485D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9713B258-6AD1-4F3D-80CC-FF9ADBD0AA95}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{AD1B03CA-9232-4F2D-A5D2-63064345160B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t>Modelo</t>
   </si>
@@ -104,15 +104,6 @@
     <t>Pronóstico</t>
   </si>
   <si>
-    <t>11 035.20</t>
-  </si>
-  <si>
-    <t>10 758.29</t>
-  </si>
-  <si>
-    <t>11 312.10</t>
-  </si>
-  <si>
     <t>11 046.09</t>
   </si>
   <si>
@@ -162,6 +153,63 @@
   </si>
   <si>
     <t>Límite superior</t>
+  </si>
+  <si>
+    <t>Periodo</t>
+  </si>
+  <si>
+    <t>10 879.75</t>
+  </si>
+  <si>
+    <t>10 650.83</t>
+  </si>
+  <si>
+    <t>11 108.66</t>
+  </si>
+  <si>
+    <t>10 853.74</t>
+  </si>
+  <si>
+    <t>10 586.44</t>
+  </si>
+  <si>
+    <t>11 121.03</t>
+  </si>
+  <si>
+    <t>10 913.53</t>
+  </si>
+  <si>
+    <t>10 612.72</t>
+  </si>
+  <si>
+    <t>11 214.33</t>
+  </si>
+  <si>
+    <t>11 023.38</t>
+  </si>
+  <si>
+    <t>10 692.43</t>
+  </si>
+  <si>
+    <t>11 354.33</t>
+  </si>
+  <si>
+    <t>11 033.29</t>
+  </si>
+  <si>
+    <t>10 674.72</t>
+  </si>
+  <si>
+    <t>11 391.85</t>
+  </si>
+  <si>
+    <t>10 940.04</t>
+  </si>
+  <si>
+    <t>10 555.84</t>
+  </si>
+  <si>
+    <t>11 324.25</t>
   </si>
 </sst>
 </file>
@@ -220,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -236,6 +284,15 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B6C11-13F9-4C03-BFC2-EFBD0D58981C}">
-  <dimension ref="C9:H37"/>
+  <dimension ref="C9:H47"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B13" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B30" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,24 +738,32 @@
         <v>21</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C32" s="5">
         <v>43647</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>24</v>
+      <c r="D32" s="4">
+        <v>11035.2</v>
+      </c>
+      <c r="E32" s="4">
+        <v>10758.29</v>
+      </c>
+      <c r="F32" s="4">
+        <v>11312.1</v>
+      </c>
+      <c r="G32">
+        <f>D32-E32</f>
+        <v>276.90999999999985</v>
+      </c>
+      <c r="H32">
+        <f>F32-D32</f>
+        <v>276.89999999999964</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.25">
@@ -706,13 +771,13 @@
         <v>43678</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
@@ -720,13 +785,13 @@
         <v>43709</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.25">
@@ -734,13 +799,13 @@
         <v>43739</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
@@ -748,13 +813,13 @@
         <v>43770</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
@@ -762,13 +827,111 @@
         <v>43800</v>
       </c>
       <c r="D37" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C41" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="F41" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>39</v>
+    </row>
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C42" s="7">
+        <v>43647</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C43" s="7">
+        <v>43678</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="7">
+        <v>43709</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="7">
+        <v>43739</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C46" s="7">
+        <v>43770</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="7">
+        <v>43800</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>